<commit_message>
add updated test file with formula bug: unsupported relationship
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/l0rda/Documents/Projects/testgooxmlinsert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689280E9-B6E6-CE46-810B-CB73AEB6A561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E681F24-1EF4-9E47-95A8-C0484BDFA9D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31960" yWindow="4700" windowWidth="27840" windowHeight="17060" xr2:uid="{D6B9B8CA-A796-774A-9345-1CD429C4BBCE}"/>
   </bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,7 +576,9 @@
       <c r="A2" s="5"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -584,7 +586,10 @@
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7">
+        <f>SUM(D2:D2)</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>